<commit_message>
Switch to new Industry Categories in 3 variables (#89)
</commit_message>
<xml_diff>
--- a/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
+++ b/InputData/indst/PPRiFUfICaWHR/Pot Perc Red in Fuel Use fr Inc Cogen and WHR.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\indst\PPRiFUfICaWHR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\indst\PPRiFUfICaWHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649E8F92-5031-4E5C-A383-AB9DE5FAA438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="11055"/>
+    <workbookView xWindow="4470" yWindow="1620" windowWidth="23580" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="PPRiFUfICaWHR" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Source:</t>
   </si>
@@ -62,46 +74,100 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>We do not apply this potential to Agriculture, due to its lack of large, heat-generating,</t>
-  </si>
-  <si>
     <t>stationary equipment compared to other industries.</t>
   </si>
   <si>
-    <t>cement and other carbonates</t>
-  </si>
-  <si>
-    <t>natural gas and petroleum systems</t>
-  </si>
-  <si>
-    <t>iron and steel</t>
-  </si>
-  <si>
-    <t>chemicals</t>
-  </si>
-  <si>
-    <t>mining</t>
-  </si>
-  <si>
-    <t>waste management</t>
-  </si>
-  <si>
-    <t>agriculture</t>
-  </si>
-  <si>
-    <t>other industries</t>
-  </si>
-  <si>
     <t>PPRiFUfICaWHR Potential Perc Reduction in Fuel Use from Increased Cogen and Waste Heat Recovery</t>
   </si>
   <si>
-    <t>Pot Perc Red in Fuel Use (dimensionless)</t>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
+  </si>
+  <si>
+    <t>Unit: dimensionless</t>
+  </si>
+  <si>
+    <t>Pot Perc Red in Fuel Use</t>
+  </si>
+  <si>
+    <t>We do not apply this potential to non-manufacturing indutries due to their lack of large, heat-generating,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -138,7 +204,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,7 +246,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -194,14 +262,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -297,6 +362,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -332,6 +414,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,23 +606,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.1328125" customWidth="1"/>
-    <col min="3" max="3" width="29.86328125" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,44 +630,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2011</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -576,18 +675,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.59765625" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -595,7 +694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -603,7 +702,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -611,7 +710,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -620,7 +719,7 @@
         <v>7.8688524590163927E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -628,7 +727,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -643,96 +742,244 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.73046875" customWidth="1"/>
-    <col min="2" max="2" width="23.73046875" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="13">
+      <c r="B11" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="10">
+        <f>Data!B$7</f>
+        <v>7.8688524590163927E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="10">
-        <f>Data!B$7</f>
-        <v>7.8688524590163927E-2</v>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>